<commit_message>
cập nhật sao kê 16/06/2025
</commit_message>
<xml_diff>
--- a/SAO KÊ/lich-su-giao-dich-tai-khoan.xlsx
+++ b/SAO KÊ/lich-su-giao-dich-tai-khoan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tungnx\Documents\NetSarang Computer\6\Xftp\Temporary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\longn\OneDrive\Máy tính\Mother\SAO KÊ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833D212D-859E-4198-BF48-6E7FEEC07B45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C8B441-1F5B-43F1-80F7-04C069FBF1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9450" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vietcombank_Account_Statement" sheetId="1" r:id="rId1"/>
@@ -19,20 +19,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Tung Nghiem Xuan</author>
-  </authors>
-  <commentList/>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="90">
-  <si>
-    <t>${cif}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="92">
   <si>
     <t>Trân trọng cảm ơn quý khách đã sử dụng dịch vụ Vietcombank!
 Thank you for using Vietcombank’s services!
@@ -84,9 +72,6 @@
     </r>
   </si>
   <si>
-    <t>${report_date}</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Chủ tài khoản/ </t>
     </r>
@@ -264,9 +249,6 @@
       </rPr>
       <t>To:</t>
     </r>
-  </si>
-  <si>
-    <t>${to_date}</t>
   </si>
   <si>
     <r>
@@ -472,57 +454,6 @@
     <t>DIGIBANK</t>
   </si>
   <si>
-    <t>${from_date}</t>
-  </si>
-  <si>
-    <t>${trans.numberOrder}</t>
-  </si>
-  <si>
-    <t>${trans.refCustom}</t>
-  </si>
-  <si>
-    <t>${trans.minusAmount}</t>
-  </si>
-  <si>
-    <t>${trans.plusAmount}</t>
-  </si>
-  <si>
-    <t>${trans.balanceAmount}</t>
-  </si>
-  <si>
-    <t>${trans.description}</t>
-  </si>
-  <si>
-    <t>${account.accountName}</t>
-  </si>
-  <si>
-    <t>${account.accountNo}</t>
-  </si>
-  <si>
-    <t>${account.accountType}</t>
-  </si>
-  <si>
-    <t>${account.accountNum}</t>
-  </si>
-  <si>
-    <t>${account.accountAddress}</t>
-  </si>
-  <si>
-    <t>${account.accountIdNumber}</t>
-  </si>
-  <si>
-    <t>${account.accountCurrency}</t>
-  </si>
-  <si>
-    <t>${totalAmount} ${account.accountCurrency}</t>
-  </si>
-  <si>
-    <t>${endAmount} ${account.accountCurrency}</t>
-  </si>
-  <si>
-    <t>${startAmount} ${account.accountCurrency}</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -548,6 +479,9 @@
   </si>
   <si>
     <t>201,880 VND</t>
+  </si>
+  <si>
+    <t>17/06/2025</t>
   </si>
   <si>
     <t>1</t>
@@ -615,7 +549,7 @@
   </si>
   <si>
     <t>16/06/2025
-5387 - 2255</t>
+5387 - 02255</t>
   </si>
   <si>
     <t>200,000</t>
@@ -631,7 +565,7 @@
   </si>
   <si>
     <t>16/06/2025
-5245 - 1215</t>
+5245 - 01215</t>
   </si>
   <si>
     <t>650,000</t>
@@ -653,18 +587,85 @@
     <t>MBVCB.9878809756.Tat ca se on thoi,co len nhe..CT tu 0391000291285 VO THI HUYNH NHI toi 1047279571 TRAN THANH HOA</t>
   </si>
   <si>
-    <t>648,120 VND</t>
-  </si>
-  <si>
-    <t>850,000 VND</t>
+    <t>8</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5239 - 07178</t>
+  </si>
+  <si>
+    <t>1,050,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9882337809.chuc bac mau khoe.CT tu 1039251552 TRAN NGOC KIM KHANH toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5244 - 15054</t>
+  </si>
+  <si>
+    <t>1,150,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9882666906.NGUYEN ANH THU chuyen tien. Mong co mau khoe.CT tu 1018320656 NGUYEN ANH THU toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5387 - 95808</t>
+  </si>
+  <si>
+    <t>1,350,000</t>
+  </si>
+  <si>
+    <t>020097041506170905132025iuP1886929.95808.090513.TRAN THU TRUC Chuyen tien cau mong Me em chong qua con bao benh nhen</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5241 - 20623</t>
+  </si>
+  <si>
+    <t>500,000</t>
+  </si>
+  <si>
+    <t>1,850,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9882893260.ANH SI PKD GUI.CT tu 1039251216 NGUYEN HUNG SI toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5389 - 29643</t>
+  </si>
+  <si>
+    <t>2,350,000</t>
+  </si>
+  <si>
+    <t>020097040506170914162025ZM9G040590.29643.091417.Vietcombank:1047279571:anh ngoc hongduc1 ho tro</t>
+  </si>
+  <si>
+    <t>2,148,120 VND</t>
+  </si>
+  <si>
+    <t>2,350,000 VND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -899,19 +900,6 @@
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1270,13 +1258,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1290,36 +1277,45 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1330,20 +1326,8 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1420,9 +1404,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>400051</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>10002</xdr:rowOff>
+      <xdr:colOff>577851</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60802</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1737,33 +1721,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="true" style="2" width="4.7109375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="2" width="6.28515625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="2" width="17.7109375" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="2" width="22.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="2" width="13.28515625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="2" width="15.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="2" width="23.85546875" collapsed="false"/>
-    <col min="8" max="16384" style="2" width="8.85546875" collapsed="false"/>
+    <col min="1" max="1" width="4.7265625" style="2" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="36.0" customHeight="true" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1"/>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="E1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -1784,10 +1770,9 @@
       <c r="Y1"/>
       <c r="Z1"/>
     </row>
-    <row r="2" spans="1:26" ht="13.9" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="3"/>
+    <row r="2" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
@@ -1808,20 +1793,20 @@
       <c r="Y2"/>
       <c r="Z2"/>
     </row>
-    <row r="3" spans="1:26" ht="30.0" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B3" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="19" t="s">
+    <row r="3" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="7" t="s">
-        <v>54</v>
+      <c r="C3" s="18"/>
+      <c r="D3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -1843,20 +1828,20 @@
       <c r="Y3"/>
       <c r="Z3"/>
     </row>
-    <row r="4" spans="1:26" ht="27.0" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="6" t="s">
+    <row r="4" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="6" t="s">
         <v>29</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
@@ -1878,20 +1863,20 @@
       <c r="Y4"/>
       <c r="Z4"/>
     </row>
-    <row r="5" spans="1:26" ht="42.0" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="6" t="s">
-        <v>56</v>
+    <row r="5" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -1913,17 +1898,17 @@
       <c r="Y5"/>
       <c r="Z5"/>
     </row>
-    <row r="6" spans="1:26" ht="13.9" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
+    <row r="6" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
@@ -1944,17 +1929,17 @@
       <c r="Y6"/>
       <c r="Z6"/>
     </row>
-    <row r="7" spans="1:26" ht="27.75" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+    <row r="7" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
@@ -1975,15 +1960,15 @@
       <c r="Y7"/>
       <c r="Z7"/>
     </row>
-    <row r="8" spans="1:26" ht="13.9" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
+    <row r="8" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
@@ -2004,17 +1989,17 @@
       <c r="Y8"/>
       <c r="Z8"/>
     </row>
-    <row r="9" spans="1:26" ht="18.0" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+    <row r="9" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
@@ -2035,21 +2020,21 @@
       <c r="Y9"/>
       <c r="Z9"/>
     </row>
-    <row r="10" spans="1:26" ht="19.5" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="19"/>
+    <row r="10" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="18"/>
       <c r="H10"/>
       <c r="I10"/>
       <c r="J10"/>
@@ -2070,17 +2055,17 @@
       <c r="Y10"/>
       <c r="Z10"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
+    <row r="11" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
@@ -2101,13 +2086,7 @@
       <c r="Y11"/>
       <c r="Z11"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+    <row r="12" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12"/>
@@ -2128,24 +2107,24 @@
       <c r="Y12"/>
       <c r="Z12"/>
     </row>
-    <row r="13" spans="1:26" ht="54.75" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="1:26" ht="42" x14ac:dyDescent="0.35">
+      <c r="B13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="F13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -2167,25 +2146,25 @@
       <c r="Y13"/>
       <c r="Z13"/>
     </row>
-    <row r="14" spans="1:26" ht="60.0" x14ac:dyDescent="0.25" customHeight="true">
+    <row r="14" spans="1:26" ht="56" x14ac:dyDescent="0.35">
       <c r="A14"/>
-      <c r="B14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>60</v>
+      <c r="B14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
@@ -2207,24 +2186,24 @@
       <c r="Y14"/>
       <c r="Z14"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25" ht="60.0" customHeight="true">
-      <c r="B15" t="s" s="13">
-        <v>61</v>
-      </c>
-      <c r="C15" t="s" s="14">
-        <v>62</v>
-      </c>
-      <c r="D15" t="s" s="16">
-        <v>47</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" t="s" s="16">
-        <v>63</v>
-      </c>
-      <c r="G15" t="s" s="15">
-        <v>64</v>
+    <row r="15" spans="1:26" ht="42" x14ac:dyDescent="0.35">
+      <c r="B15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -2246,24 +2225,24 @@
       <c r="Y15"/>
       <c r="Z15"/>
     </row>
-    <row r="16" spans="1:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="16" t="s">
+    <row r="16" spans="1:26" ht="42" x14ac:dyDescent="0.35">
+      <c r="B16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>69</v>
+      <c r="D16" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="H16"/>
       <c r="I16"/>
@@ -2285,24 +2264,24 @@
       <c r="Y16"/>
       <c r="Z16"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25" ht="60.0" customHeight="true">
-      <c r="B17" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>74</v>
+    <row r="17" spans="2:26" ht="56" x14ac:dyDescent="0.35">
+      <c r="B17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="H17"/>
       <c r="I17"/>
@@ -2324,24 +2303,24 @@
       <c r="Y17"/>
       <c r="Z17"/>
     </row>
-    <row r="18" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>79</v>
+    <row r="18" spans="2:26" ht="42" x14ac:dyDescent="0.35">
+      <c r="B18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="H18"/>
       <c r="I18"/>
@@ -2363,24 +2342,24 @@
       <c r="Y18"/>
       <c r="Z18"/>
     </row>
-    <row r="19" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>83</v>
+    <row r="19" spans="2:26" ht="42" x14ac:dyDescent="0.35">
+      <c r="B19" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -2402,24 +2381,24 @@
       <c r="Y19"/>
       <c r="Z19"/>
     </row>
-    <row r="20" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>87</v>
+    <row r="20" spans="2:26" ht="56" x14ac:dyDescent="0.35">
+      <c r="B20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
@@ -2441,13 +2420,25 @@
       <c r="Y20"/>
       <c r="Z20"/>
     </row>
-    <row r="21" spans="2:26" ht="15.0" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="D21" s="0"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="0"/>
-      <c r="G21" s="0"/>
+    <row r="21" spans="2:26" ht="56" x14ac:dyDescent="0.35">
+      <c r="B21" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -2468,17 +2459,25 @@
       <c r="Y21"/>
       <c r="Z21"/>
     </row>
-    <row r="22" spans="2:26" ht="19.5" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B22" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
+    <row r="22" spans="2:26" ht="56" x14ac:dyDescent="0.35">
+      <c r="B22" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -2499,17 +2498,25 @@
       <c r="Y22"/>
       <c r="Z22"/>
     </row>
-    <row r="23" spans="2:26" ht="15.0" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
+    <row r="23" spans="2:26" ht="56" x14ac:dyDescent="0.35">
+      <c r="B23" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>80</v>
+      </c>
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
@@ -2530,13 +2537,25 @@
       <c r="Y23"/>
       <c r="Z23"/>
     </row>
-    <row r="24" spans="2:26" ht="10.5" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+    <row r="24" spans="2:26" ht="42" x14ac:dyDescent="0.35">
+      <c r="B24" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -2557,15 +2576,25 @@
       <c r="Y24"/>
       <c r="Z24"/>
     </row>
-    <row r="25" spans="2:26" s="5" customFormat="1" ht="16.9" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
+    <row r="25" spans="2:26" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="B25" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
@@ -2586,13 +2615,13 @@
       <c r="Y25"/>
       <c r="Z25"/>
     </row>
-    <row r="26" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25" ht="13.9" customHeight="true">
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
+    <row r="26" spans="2:26" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26" s="3"/>
+      <c r="F26"/>
+      <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
@@ -2613,11 +2642,15 @@
       <c r="Y26"/>
       <c r="Z26"/>
     </row>
-    <row r="27" spans="2:26" ht="21.0" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+    <row r="27" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="21" t="s">
+        <v>90</v>
+      </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
       <c r="H27"/>
@@ -2640,15 +2673,17 @@
       <c r="Y27"/>
       <c r="Z27"/>
     </row>
-    <row r="28" spans="2:26" ht="13.9" customHeight="true" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
+    <row r="28" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B28" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
@@ -2669,13 +2704,13 @@
       <c r="Y28"/>
       <c r="Z28"/>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25" ht="18.0" customHeight="true">
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
+    <row r="29" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
@@ -2696,13 +2731,15 @@
       <c r="Y29"/>
       <c r="Z29"/>
     </row>
-    <row r="30" spans="2:26" x14ac:dyDescent="0.25" ht="12.0" customHeight="true">
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
+    <row r="30" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
@@ -2723,15 +2760,13 @@
       <c r="Y30"/>
       <c r="Z30"/>
     </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.25" ht="13.15" customHeight="true">
-      <c r="B31" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+    <row r="31" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
@@ -2752,13 +2787,13 @@
       <c r="Y31"/>
       <c r="Z31"/>
     </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.25" ht="15.0" customHeight="true">
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+    <row r="32" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
@@ -2779,83 +2814,118 @@
       <c r="Y32"/>
       <c r="Z32"/>
     </row>
-    <row r="33" ht="26.25" customHeight="true">
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-    </row>
-    <row r="34" ht="8.25" customHeight="true">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" ht="15.0" customHeight="true">
-      <c r="B35" t="s" s="19">
-        <v>22</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-    </row>
-    <row r="36" ht="15.0" customHeight="true">
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-    </row>
-    <row r="37" ht="15.0" customHeight="true">
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="B40:G42"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B30:G32"/>
+    <mergeCell ref="B33:G35"/>
+    <mergeCell ref="B36:G38"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:G27"/>
-    <mergeCell ref="B28:G30"/>
-    <mergeCell ref="B31:G33"/>
-    <mergeCell ref="B35:G37"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add sao kê 17, 18, 19
</commit_message>
<xml_diff>
--- a/SAO KÊ/lich-su-giao-dich-tai-khoan.xlsx
+++ b/SAO KÊ/lich-su-giao-dich-tai-khoan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\longn\OneDrive\Máy tính\Mother\SAO KÊ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tungnx\Documents\NetSarang Computer\6\Xftp\Temporary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C8B441-1F5B-43F1-80F7-04C069FBF1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833D212D-859E-4198-BF48-6E7FEEC07B45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="9450" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vietcombank_Account_Statement" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,20 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tung Nghiem Xuan</author>
+  </authors>
+  <commentList/>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="303">
+  <si>
+    <t>${cif}</t>
+  </si>
   <si>
     <t>Trân trọng cảm ơn quý khách đã sử dụng dịch vụ Vietcombank!
 Thank you for using Vietcombank’s services!
@@ -72,6 +84,9 @@
     </r>
   </si>
   <si>
+    <t>${report_date}</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Chủ tài khoản/ </t>
     </r>
@@ -249,6 +264,9 @@
       </rPr>
       <t>To:</t>
     </r>
+  </si>
+  <si>
+    <t>${to_date}</t>
   </si>
   <si>
     <r>
@@ -454,6 +472,57 @@
     <t>DIGIBANK</t>
   </si>
   <si>
+    <t>${from_date}</t>
+  </si>
+  <si>
+    <t>${trans.numberOrder}</t>
+  </si>
+  <si>
+    <t>${trans.refCustom}</t>
+  </si>
+  <si>
+    <t>${trans.minusAmount}</t>
+  </si>
+  <si>
+    <t>${trans.plusAmount}</t>
+  </si>
+  <si>
+    <t>${trans.balanceAmount}</t>
+  </si>
+  <si>
+    <t>${trans.description}</t>
+  </si>
+  <si>
+    <t>${account.accountName}</t>
+  </si>
+  <si>
+    <t>${account.accountNo}</t>
+  </si>
+  <si>
+    <t>${account.accountType}</t>
+  </si>
+  <si>
+    <t>${account.accountNum}</t>
+  </si>
+  <si>
+    <t>${account.accountAddress}</t>
+  </si>
+  <si>
+    <t>${account.accountIdNumber}</t>
+  </si>
+  <si>
+    <t>${account.accountCurrency}</t>
+  </si>
+  <si>
+    <t>${totalAmount} ${account.accountCurrency}</t>
+  </si>
+  <si>
+    <t>${endAmount} ${account.accountCurrency}</t>
+  </si>
+  <si>
+    <t>${startAmount} ${account.accountCurrency}</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -481,7 +550,7 @@
     <t>201,880 VND</t>
   </si>
   <si>
-    <t>17/06/2025</t>
+    <t>20/06/2025</t>
   </si>
   <si>
     <t>1</t>
@@ -655,17 +724,636 @@
     <t>020097040506170914162025ZM9G040590.29643.091417.Vietcombank:1047279571:anh ngoc hongduc1 ho tro</t>
   </si>
   <si>
-    <t>2,148,120 VND</t>
-  </si>
-  <si>
-    <t>2,350,000 VND</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5240 - 71430</t>
+  </si>
+  <si>
+    <t>2,450,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9884742574.VO VAN HAU chuyen tien.CT tu 1039251827 VO VAN HAU toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5212 - 69204</t>
+  </si>
+  <si>
+    <t>2,550,000</t>
+  </si>
+  <si>
+    <t>007400.170625.115107.IBFT Nhi can tin h6 gui quy ung ho</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5239 - 87696</t>
+  </si>
+  <si>
+    <t>2,750,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9885314525.PHUNG MINH SON chuyen tien.CT tu 0111000220233 PHUNG MINH SON toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5209 - 46678</t>
+  </si>
+  <si>
+    <t>300,000</t>
+  </si>
+  <si>
+    <t>3,050,000</t>
+  </si>
+  <si>
+    <t>356703.170625.132858.Pham Xuan Hoa chuyen tien</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5213 - 58524</t>
+  </si>
+  <si>
+    <t>3,250,000</t>
+  </si>
+  <si>
+    <t>214672.170625.133354.IBFT HUYNH THI DIEM TRANG chuyen tien- gd co len nha</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5217 - 56497</t>
+  </si>
+  <si>
+    <t>3,350,000</t>
+  </si>
+  <si>
+    <t>990157.170625.141146.VO THI DIEU HIEN - KE TOAN H6 - HO TRO MONG ME CUNG MAU KHOE</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5017 - 57985</t>
+  </si>
+  <si>
+    <t>3,450,000</t>
+  </si>
+  <si>
+    <t>143323.170625.141209.Ke toan H6 gui ung ho</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5389 - 92010</t>
+  </si>
+  <si>
+    <t>3,650,000</t>
+  </si>
+  <si>
+    <t>020097041506171452572025uXK8923426.92010.145249.Mong me anh mau khoi benh va manh khoe</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5220 - 16424</t>
+  </si>
+  <si>
+    <t>2,100,000</t>
+  </si>
+  <si>
+    <t>5,750,000</t>
+  </si>
+  <si>
+    <t>412383.170625.150647.IBFT HDMT gui em</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5212 - 57443</t>
+  </si>
+  <si>
+    <t>6,800,000</t>
+  </si>
+  <si>
+    <t>314764.170625.151948.Hdlt gui Hoa</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5219 - 65844</t>
+  </si>
+  <si>
+    <t>6,900,000</t>
+  </si>
+  <si>
+    <t>444057.170625.152233.IBFT NGUYEN THI YEN NHI</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5243 - 29784</t>
+  </si>
+  <si>
+    <t>7,100,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9886795257.NGUYEN THI KIM XUYEN chuyen tien.CT tu 1016421826 NGUYEN THI KIM XUYEN toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5240 - 41500</t>
+  </si>
+  <si>
+    <t>7,150,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9887196366.THAI VINH HUY chuyen tien.CT tu 9388319165 THAI VINH HUY toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5216 - 36434</t>
+  </si>
+  <si>
+    <t>2,900,000</t>
+  </si>
+  <si>
+    <t>10,050,000</t>
+  </si>
+  <si>
+    <t>638520.170625.164306.IBFT Tap the hong duc 2 chuyen tien</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>17/06/2025
+5220 - 04549</t>
+  </si>
+  <si>
+    <t>10,250,000</t>
+  </si>
+  <si>
+    <t>277349.170625.210311.IBFT HO THI THIEN KIM hong duc 3 gui it long</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>18/06/2025
+5387 - 71804</t>
+  </si>
+  <si>
+    <t>10,750,000</t>
+  </si>
+  <si>
+    <t>0200970415061807213520259kQi954236.71804.072135.QR - e xin gop it suc cung gia dinh a</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>18/06/2025
+5218 - 39323</t>
+  </si>
+  <si>
+    <t>10,950,000</t>
+  </si>
+  <si>
+    <t>708724.180625.075824.IBFT  Ck</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>18/06/2025
+5241 - 48326</t>
+  </si>
+  <si>
+    <t>11,150,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9894767059.PHAN TIEN TAI -1921 PHAM HOAI NHAN -1684.CT tu 1048009183 PHAN TIEN TAI toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>18/06/2025
+5216 - 75304</t>
+  </si>
+  <si>
+    <t>11,250,000</t>
+  </si>
+  <si>
+    <t>112046.180625.111100.IBFT Cua it long nhiu nhe Hoa - chuc cho moi thu tot dep hon nha</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>18/06/2025
+5161 - 25501</t>
+  </si>
+  <si>
+    <t>11,350,000</t>
+  </si>
+  <si>
+    <t>PARTNER.DIRECT_DEBITS_VCB.MSE.91214874852.20250618.91214874852-0845627828_TRUONG HUYNH NHU chuyen tien qua MoMo</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>18/06/2025
+5216 - 32869</t>
+  </si>
+  <si>
+    <t>3,200,000</t>
+  </si>
+  <si>
+    <t>14,550,000</t>
+  </si>
+  <si>
+    <t>362096.180625.130554.IBFT PTCKT ho tro Gd Tran Thanh Hoa</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>18/06/2025
+5240 - 14741</t>
+  </si>
+  <si>
+    <t>20,300,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9897080704.LE THI KIM THANH chuyen tien.CT tu 0111000168989 LE THI KIM THANH toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>18/06/2025
+5078 - 58506</t>
+  </si>
+  <si>
+    <t>20,600,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9897199882.VO MINH SON chuyen tien.CT tu 1039251219 VO MINH SON toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>18/06/2025
+5243 - 51997</t>
+  </si>
+  <si>
+    <t>20,650,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9898356501.My Duyen Hong 6 chuc me anh mau het benh.CT tu 1028350595 HOANG THI MY DUYEN toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5219 - 47212</t>
+  </si>
+  <si>
+    <t>20,750,000</t>
+  </si>
+  <si>
+    <t>904711.190625.080610.IBFT  NHUNG tiep nhan h3</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5240 - 31429</t>
+  </si>
+  <si>
+    <t>400,000</t>
+  </si>
+  <si>
+    <t>21,150,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9904890125.Chau Dat NVBH HD4 gui anh. Chuc me anh mau khoe!.CT tu 0111001113148 CHAU THANH DAT toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5220 - 19061</t>
+  </si>
+  <si>
+    <t>21,200,000</t>
+  </si>
+  <si>
+    <t>907622.190625.102711.LE THI KIM XOAN chuyen tien</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5239 - 67436</t>
+  </si>
+  <si>
+    <t>21,300,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9906267089.NGAN TAM HD6.CT tu 1039252102 LE NGAN TAM toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5189 - 44619</t>
+  </si>
+  <si>
+    <t>21,500,000</t>
+  </si>
+  <si>
+    <t>020097041506191039062025S0Q4876305.44619.103906.QR - TRAN THI DIEM MY H12 gop suc cung gd anh</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5078 - 50966</t>
+  </si>
+  <si>
+    <t>1,250,000</t>
+  </si>
+  <si>
+    <t>22,750,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9906623783.Dai dien CH NCT goi ung ho.CT tu 0111000842614 LE TUAN KIET toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5212 - 60085</t>
+  </si>
+  <si>
+    <t>22,850,000</t>
+  </si>
+  <si>
+    <t>424538.190625.121028.IBFT Tiep nhan h9</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5216 - 81980</t>
+  </si>
+  <si>
+    <t>2,700,000</t>
+  </si>
+  <si>
+    <t>25,550,000</t>
+  </si>
+  <si>
+    <t>728774.190625.144631.IBFT Hong duc 9 chuyen tien</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5388 - 06368</t>
+  </si>
+  <si>
+    <t>1,700,000</t>
+  </si>
+  <si>
+    <t>27,250,000</t>
+  </si>
+  <si>
+    <t>0200970415061916593920253fup992293.6368.165939.QR - Hong duc 12 chuyen tien ho tro</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5239 - 84342</t>
+  </si>
+  <si>
+    <t>27,750,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9910334287.TRAN DANG KHOA CHT HD6 gui tien ho tro.CT tu 1020525485 TRAN DANG KHOA toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5218 - 16890</t>
+  </si>
+  <si>
+    <t>27,850,000</t>
+  </si>
+  <si>
+    <t>116681.190625.172927.IBFT NGUYEN THI BICH TUYEN HD6</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>19/06/2025
+5017 - 52387</t>
+  </si>
+  <si>
+    <t>28,150,000</t>
+  </si>
+  <si>
+    <t>142526.190625.173911.IBFT An trieu ban hang h10 xin phep ho tro anh</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>20/06/2025
+5215 - 31006</t>
+  </si>
+  <si>
+    <t>28,200,000</t>
+  </si>
+  <si>
+    <t>971994.200625.070614.IBFT Di 3 H6 gui quy ung ho</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>20/06/2025
+5389 - 65951</t>
+  </si>
+  <si>
+    <t>28,650,000</t>
+  </si>
+  <si>
+    <t>020097041506200753452025NKaV645869.65951.075335.QR - Hong duc 12 chuyen tien ho tro dot 2</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>20/06/2025
+9920 - 00488</t>
+  </si>
+  <si>
+    <t>1,543,501</t>
+  </si>
+  <si>
+    <t>30,193,501</t>
+  </si>
+  <si>
+    <t>IBVCB.202506205087045740.488.Thanh toan tien luong DS thang 5.2025</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>20/06/2025
+5282 - 66689</t>
+  </si>
+  <si>
+    <t>MBVCB.9916680902.803832.TRAN THANH HOA chuyen tien.CT tu 1047279571 TRAN THANH HOA toi 7411065146 TRAN THANH HOA tai BIDV</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>20/06/2025
+5388 - 92422</t>
+  </si>
+  <si>
+    <t>29,150,000</t>
+  </si>
+  <si>
+    <t>020097041506200931002025s1pB903296.92422.093050.QR - LE MINH NGOC HD5 gui chut long thanh</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>20/06/2025
+5239 - 59243</t>
+  </si>
+  <si>
+    <t>1,000,000</t>
+  </si>
+  <si>
+    <t>30,150,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9916785297.NGUYEN THI RUOI chuyen tien.CT tu 1039251871 NGUYEN THI RUOI toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>20/06/2025
+5244 - 61023</t>
+  </si>
+  <si>
+    <t>30,450,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9916852451.Mr Thuc gui Hoa chuc bac mau khoe.CT tu 1039252667 LE CHINH THUC toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>20/06/2025
+5241 - 64985</t>
+  </si>
+  <si>
+    <t>600,000</t>
+  </si>
+  <si>
+    <t>31,050,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9916998233.LE THI KIM THANH chuyen tien.CT tu 0111000168989 LE THI KIM THANH toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>20/06/2025
+5241 - 72631</t>
+  </si>
+  <si>
+    <t>700,000</t>
+  </si>
+  <si>
+    <t>31,750,000</t>
+  </si>
+  <si>
+    <t>MBVCB.9917258916.Tap the Hoa Duc ST chuyen tien ho tro.CT tu 1039251865 NGUYEN HOANG THANH NGOC toi 1047279571 TRAN THANH HOA</t>
+  </si>
+  <si>
+    <t>31,548,120 VND</t>
+  </si>
+  <si>
+    <t>31,750,000 VND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -900,6 +1588,19 @@
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1258,12 +1959,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1277,45 +1979,36 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1326,8 +2019,20 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1404,9 +2109,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>577851</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>60802</xdr:rowOff>
+      <xdr:colOff>400051</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>10002</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1721,35 +2426,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="2" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.81640625" style="2"/>
+    <col min="1" max="1" customWidth="true" hidden="true" style="2" width="4.7109375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="2" width="6.28515625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="2" width="17.7109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="2" width="22.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="2" width="13.28515625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="2" width="15.0" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="2" width="23.85546875" collapsed="false"/>
+    <col min="8" max="16384" style="2" width="8.85546875" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="36.0" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="E1" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -1770,9 +2473,10 @@
       <c r="Y1"/>
       <c r="Z1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+    <row r="2" spans="1:26" ht="13.9" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="3"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
@@ -1793,20 +2497,20 @@
       <c r="Y2"/>
       <c r="Z2"/>
     </row>
-    <row r="3" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="18" t="s">
+    <row r="3" spans="1:26" ht="30.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="6" t="s">
-        <v>36</v>
+      <c r="F3" s="19"/>
+      <c r="G3" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -1828,20 +2532,20 @@
       <c r="Y3"/>
       <c r="Z3"/>
     </row>
-    <row r="4" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="6" t="s">
+    <row r="4" spans="1:26" ht="27.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
@@ -1863,20 +2567,20 @@
       <c r="Y4"/>
       <c r="Z4"/>
     </row>
-    <row r="5" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="5" t="s">
-        <v>37</v>
+    <row r="5" spans="1:26" ht="42.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -1898,17 +2602,17 @@
       <c r="Y5"/>
       <c r="Z5"/>
     </row>
-    <row r="6" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+    <row r="6" spans="1:26" ht="13.9" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
@@ -1929,17 +2633,17 @@
       <c r="Y6"/>
       <c r="Z6"/>
     </row>
-    <row r="7" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
+    <row r="7" spans="1:26" ht="27.75" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
@@ -1960,15 +2664,15 @@
       <c r="Y7"/>
       <c r="Z7"/>
     </row>
-    <row r="8" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+    <row r="8" spans="1:26" ht="13.9" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
@@ -1989,17 +2693,17 @@
       <c r="Y8"/>
       <c r="Z8"/>
     </row>
-    <row r="9" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+    <row r="9" spans="1:26" ht="18.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
@@ -2020,21 +2724,21 @@
       <c r="Y9"/>
       <c r="Z9"/>
     </row>
-    <row r="10" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="18"/>
+    <row r="10" spans="1:26" ht="19.5" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="19"/>
       <c r="H10"/>
       <c r="I10"/>
       <c r="J10"/>
@@ -2055,17 +2759,17 @@
       <c r="Y10"/>
       <c r="Z10"/>
     </row>
-    <row r="11" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
+    <row r="11" spans="1:26" ht="15.75" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
@@ -2086,7 +2790,13 @@
       <c r="Y11"/>
       <c r="Z11"/>
     </row>
-    <row r="12" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" ht="15.75" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12"/>
@@ -2107,24 +2817,24 @@
       <c r="Y12"/>
       <c r="Z12"/>
     </row>
-    <row r="13" spans="1:26" ht="42" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="9" t="s">
+    <row r="13" spans="1:26" ht="54.75" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="C13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="D13" s="10" t="s">
         <v>25</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -2146,25 +2856,25 @@
       <c r="Y13"/>
       <c r="Z13"/>
     </row>
-    <row r="14" spans="1:26" ht="56" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="60.0" x14ac:dyDescent="0.25" customHeight="true">
       <c r="A14"/>
-      <c r="B14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>41</v>
+      <c r="B14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
@@ -2186,24 +2896,24 @@
       <c r="Y14"/>
       <c r="Z14"/>
     </row>
-    <row r="15" spans="1:26" ht="42" x14ac:dyDescent="0.35">
-      <c r="B15" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>45</v>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25" ht="60.0" customHeight="true">
+      <c r="B15" t="s" s="13">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s" s="14">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s" s="16">
+        <v>64</v>
+      </c>
+      <c r="G15" t="s" s="15">
+        <v>65</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -2225,24 +2935,24 @@
       <c r="Y15"/>
       <c r="Z15"/>
     </row>
-    <row r="16" spans="1:26" ht="42" x14ac:dyDescent="0.35">
-      <c r="B16" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>50</v>
+    <row r="16" spans="1:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="H16"/>
       <c r="I16"/>
@@ -2264,24 +2974,24 @@
       <c r="Y16"/>
       <c r="Z16"/>
     </row>
-    <row r="17" spans="2:26" ht="56" x14ac:dyDescent="0.35">
-      <c r="B17" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>55</v>
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25" ht="60.0" customHeight="true">
+      <c r="B17" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="H17"/>
       <c r="I17"/>
@@ -2303,24 +3013,24 @@
       <c r="Y17"/>
       <c r="Z17"/>
     </row>
-    <row r="18" spans="2:26" ht="42" x14ac:dyDescent="0.35">
-      <c r="B18" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>60</v>
+    <row r="18" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="H18"/>
       <c r="I18"/>
@@ -2342,24 +3052,24 @@
       <c r="Y18"/>
       <c r="Z18"/>
     </row>
-    <row r="19" spans="2:26" ht="42" x14ac:dyDescent="0.35">
-      <c r="B19" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>64</v>
+    <row r="19" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -2381,24 +3091,24 @@
       <c r="Y19"/>
       <c r="Z19"/>
     </row>
-    <row r="20" spans="2:26" ht="56" x14ac:dyDescent="0.35">
-      <c r="B20" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>68</v>
+    <row r="20" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>88</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
@@ -2420,24 +3130,24 @@
       <c r="Y20"/>
       <c r="Z20"/>
     </row>
-    <row r="21" spans="2:26" ht="56" x14ac:dyDescent="0.35">
-      <c r="B21" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>72</v>
+    <row r="21" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
@@ -2459,24 +3169,24 @@
       <c r="Y21"/>
       <c r="Z21"/>
     </row>
-    <row r="22" spans="2:26" ht="56" x14ac:dyDescent="0.35">
-      <c r="B22" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>76</v>
+    <row r="22" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>96</v>
       </c>
       <c r="H22"/>
       <c r="I22"/>
@@ -2498,24 +3208,24 @@
       <c r="Y22"/>
       <c r="Z22"/>
     </row>
-    <row r="23" spans="2:26" ht="56" x14ac:dyDescent="0.35">
-      <c r="B23" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="12" t="s">
+    <row r="23" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>80</v>
+      <c r="F23" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>100</v>
       </c>
       <c r="H23"/>
       <c r="I23"/>
@@ -2537,24 +3247,24 @@
       <c r="Y23"/>
       <c r="Z23"/>
     </row>
-    <row r="24" spans="2:26" ht="42" x14ac:dyDescent="0.35">
-      <c r="B24" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>85</v>
+    <row r="24" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>105</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -2576,24 +3286,24 @@
       <c r="Y24"/>
       <c r="Z24"/>
     </row>
-    <row r="25" spans="2:26" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="B25" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>89</v>
+    <row r="25" spans="2:26" s="5" customFormat="1" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>109</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -2615,13 +3325,25 @@
       <c r="Y25"/>
       <c r="Z25"/>
     </row>
-    <row r="26" spans="2:26" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26" s="3"/>
-      <c r="F26"/>
-      <c r="G26"/>
+    <row r="26" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.25" ht="60.0" customHeight="true">
+      <c r="B26" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>113</v>
+      </c>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
@@ -2642,17 +3364,25 @@
       <c r="Y26"/>
       <c r="Z26"/>
     </row>
-    <row r="27" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B27" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
+    <row r="27" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B27" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>117</v>
+      </c>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -2673,17 +3403,25 @@
       <c r="Y27"/>
       <c r="Z27"/>
     </row>
-    <row r="28" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B28" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
+    <row r="28" spans="2:26" ht="60.0" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B28" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>121</v>
+      </c>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
@@ -2704,13 +3442,25 @@
       <c r="Y28"/>
       <c r="Z28"/>
     </row>
-    <row r="29" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
+    <row r="29" spans="2:26" x14ac:dyDescent="0.25" ht="60.0" customHeight="true">
+      <c r="B29" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>126</v>
+      </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
@@ -2731,15 +3481,25 @@
       <c r="Y29"/>
       <c r="Z29"/>
     </row>
-    <row r="30" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B30" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
+    <row r="30" spans="2:26" x14ac:dyDescent="0.25" ht="60.0" customHeight="true">
+      <c r="B30" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>130</v>
+      </c>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
@@ -2760,13 +3520,25 @@
       <c r="Y30"/>
       <c r="Z30"/>
     </row>
-    <row r="31" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
+    <row r="31" spans="2:26" x14ac:dyDescent="0.25" ht="60.0" customHeight="true">
+      <c r="B31" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>134</v>
+      </c>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
@@ -2787,13 +3559,25 @@
       <c r="Y31"/>
       <c r="Z31"/>
     </row>
-    <row r="32" spans="2:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
+    <row r="32" spans="2:26" x14ac:dyDescent="0.25" ht="60.0" customHeight="true">
+      <c r="B32" t="s" s="13">
+        <v>135</v>
+      </c>
+      <c r="C32" t="s" s="14">
+        <v>136</v>
+      </c>
+      <c r="D32" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E32" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="F32" t="s" s="16">
+        <v>137</v>
+      </c>
+      <c r="G32" t="s" s="15">
+        <v>138</v>
+      </c>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
@@ -2814,118 +3598,948 @@
       <c r="Y32"/>
       <c r="Z32"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="24" t="s">
+    <row r="33" ht="60.0" customHeight="true">
+      <c r="B33" t="s" s="13">
+        <v>139</v>
+      </c>
+      <c r="C33" t="s" s="14">
+        <v>140</v>
+      </c>
+      <c r="D33" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E33" t="s" s="17">
+        <v>78</v>
+      </c>
+      <c r="F33" t="s" s="16">
+        <v>141</v>
+      </c>
+      <c r="G33" t="s" s="15">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" ht="60.0" customHeight="true">
+      <c r="B34" t="s" s="13">
+        <v>143</v>
+      </c>
+      <c r="C34" t="s" s="14">
+        <v>144</v>
+      </c>
+      <c r="D34" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E34" t="s" s="17">
+        <v>145</v>
+      </c>
+      <c r="F34" t="s" s="16">
+        <v>146</v>
+      </c>
+      <c r="G34" t="s" s="15">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" ht="60.0" customHeight="true">
+      <c r="B35" t="s" s="13">
+        <v>148</v>
+      </c>
+      <c r="C35" t="s" s="14">
+        <v>149</v>
+      </c>
+      <c r="D35" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E35" t="s" s="17">
+        <v>91</v>
+      </c>
+      <c r="F35" t="s" s="16">
+        <v>150</v>
+      </c>
+      <c r="G35" t="s" s="15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" ht="60.0" customHeight="true">
+      <c r="B36" t="s" s="13">
+        <v>152</v>
+      </c>
+      <c r="C36" t="s" s="14">
+        <v>153</v>
+      </c>
+      <c r="D36" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E36" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="F36" t="s" s="16">
+        <v>154</v>
+      </c>
+      <c r="G36" t="s" s="15">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" ht="60.0" customHeight="true">
+      <c r="B37" t="s" s="13">
+        <v>156</v>
+      </c>
+      <c r="C37" t="s" s="14">
+        <v>157</v>
+      </c>
+      <c r="D37" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E37" t="s" s="17">
+        <v>78</v>
+      </c>
+      <c r="F37" t="s" s="16">
+        <v>158</v>
+      </c>
+      <c r="G37" t="s" s="15">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" ht="60.0" customHeight="true">
+      <c r="B38" t="s" s="13">
+        <v>160</v>
+      </c>
+      <c r="C38" t="s" s="14">
+        <v>161</v>
+      </c>
+      <c r="D38" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E38" t="s" s="17">
+        <v>68</v>
+      </c>
+      <c r="F38" t="s" s="16">
+        <v>162</v>
+      </c>
+      <c r="G38" t="s" s="15">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" ht="60.0" customHeight="true">
+      <c r="B39" t="s" s="13">
+        <v>164</v>
+      </c>
+      <c r="C39" t="s" s="14">
+        <v>165</v>
+      </c>
+      <c r="D39" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E39" t="s" s="17">
+        <v>166</v>
+      </c>
+      <c r="F39" t="s" s="16">
+        <v>167</v>
+      </c>
+      <c r="G39" t="s" s="15">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" ht="60.0" customHeight="true">
+      <c r="B40" t="s" s="13">
+        <v>169</v>
+      </c>
+      <c r="C40" t="s" s="14">
+        <v>170</v>
+      </c>
+      <c r="D40" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E40" t="s" s="17">
+        <v>78</v>
+      </c>
+      <c r="F40" t="s" s="16">
+        <v>171</v>
+      </c>
+      <c r="G40" t="s" s="15">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" ht="60.0" customHeight="true">
+      <c r="B41" t="s" s="13">
+        <v>173</v>
+      </c>
+      <c r="C41" t="s" s="14">
+        <v>174</v>
+      </c>
+      <c r="D41" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E41" t="s" s="17">
+        <v>103</v>
+      </c>
+      <c r="F41" t="s" s="16">
+        <v>175</v>
+      </c>
+      <c r="G41" t="s" s="15">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" ht="60.0" customHeight="true">
+      <c r="B42" t="s" s="13">
+        <v>177</v>
+      </c>
+      <c r="C42" t="s" s="14">
+        <v>178</v>
+      </c>
+      <c r="D42" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E42" t="s" s="17">
+        <v>78</v>
+      </c>
+      <c r="F42" t="s" s="16">
+        <v>179</v>
+      </c>
+      <c r="G42" t="s" s="15">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" ht="60.0" customHeight="true">
+      <c r="B43" t="s" s="13">
+        <v>181</v>
+      </c>
+      <c r="C43" t="s" s="14">
+        <v>182</v>
+      </c>
+      <c r="D43" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E43" t="s" s="17">
+        <v>78</v>
+      </c>
+      <c r="F43" t="s" s="16">
+        <v>183</v>
+      </c>
+      <c r="G43" t="s" s="15">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="44" ht="60.0" customHeight="true">
+      <c r="B44" t="s" s="13">
+        <v>185</v>
+      </c>
+      <c r="C44" t="s" s="14">
+        <v>186</v>
+      </c>
+      <c r="D44" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E44" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="F44" t="s" s="16">
+        <v>187</v>
+      </c>
+      <c r="G44" t="s" s="15">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45" ht="60.0" customHeight="true">
+      <c r="B45" t="s" s="13">
+        <v>189</v>
+      </c>
+      <c r="C45" t="s" s="14">
+        <v>190</v>
+      </c>
+      <c r="D45" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E45" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="F45" t="s" s="16">
+        <v>191</v>
+      </c>
+      <c r="G45" t="s" s="15">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" ht="60.0" customHeight="true">
+      <c r="B46" t="s" s="13">
+        <v>193</v>
+      </c>
+      <c r="C46" t="s" s="14">
+        <v>194</v>
+      </c>
+      <c r="D46" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E46" t="s" s="17">
+        <v>195</v>
+      </c>
+      <c r="F46" t="s" s="16">
+        <v>196</v>
+      </c>
+      <c r="G46" t="s" s="15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="47" ht="60.0" customHeight="true">
+      <c r="B47" t="s" s="13">
+        <v>198</v>
+      </c>
+      <c r="C47" t="s" s="14">
+        <v>199</v>
+      </c>
+      <c r="D47" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E47" t="s" s="17">
+        <v>146</v>
+      </c>
+      <c r="F47" t="s" s="16">
+        <v>200</v>
+      </c>
+      <c r="G47" t="s" s="15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" ht="60.0" customHeight="true">
+      <c r="B48" t="s" s="13">
+        <v>202</v>
+      </c>
+      <c r="C48" t="s" s="14">
+        <v>203</v>
+      </c>
+      <c r="D48" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E48" t="s" s="17">
+        <v>124</v>
+      </c>
+      <c r="F48" t="s" s="16">
+        <v>204</v>
+      </c>
+      <c r="G48" t="s" s="15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" ht="60.0" customHeight="true">
+      <c r="B49" t="s" s="13">
+        <v>206</v>
+      </c>
+      <c r="C49" t="s" s="14">
+        <v>207</v>
+      </c>
+      <c r="D49" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E49" t="s" s="17">
+        <v>68</v>
+      </c>
+      <c r="F49" t="s" s="16">
+        <v>208</v>
+      </c>
+      <c r="G49" t="s" s="15">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" ht="60.0" customHeight="true">
+      <c r="B50" t="s" s="13">
+        <v>210</v>
+      </c>
+      <c r="C50" t="s" s="14">
+        <v>211</v>
+      </c>
+      <c r="D50" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E50" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="F50" t="s" s="16">
+        <v>212</v>
+      </c>
+      <c r="G50" t="s" s="15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" ht="60.0" customHeight="true">
+      <c r="B51" t="s" s="13">
+        <v>214</v>
+      </c>
+      <c r="C51" t="s" s="14">
+        <v>215</v>
+      </c>
+      <c r="D51" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E51" t="s" s="17">
+        <v>216</v>
+      </c>
+      <c r="F51" t="s" s="16">
+        <v>217</v>
+      </c>
+      <c r="G51" t="s" s="15">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" ht="60.0" customHeight="true">
+      <c r="B52" t="s" s="13">
+        <v>219</v>
+      </c>
+      <c r="C52" t="s" s="14">
+        <v>220</v>
+      </c>
+      <c r="D52" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E52" t="s" s="17">
+        <v>68</v>
+      </c>
+      <c r="F52" t="s" s="16">
+        <v>221</v>
+      </c>
+      <c r="G52" t="s" s="15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="53" ht="60.0" customHeight="true">
+      <c r="B53" t="s" s="13">
+        <v>223</v>
+      </c>
+      <c r="C53" t="s" s="14">
+        <v>224</v>
+      </c>
+      <c r="D53" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E53" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="F53" t="s" s="16">
+        <v>225</v>
+      </c>
+      <c r="G53" t="s" s="15">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="54" ht="60.0" customHeight="true">
+      <c r="B54" t="s" s="13">
+        <v>227</v>
+      </c>
+      <c r="C54" t="s" s="14">
+        <v>228</v>
+      </c>
+      <c r="D54" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E54" t="s" s="17">
+        <v>78</v>
+      </c>
+      <c r="F54" t="s" s="16">
+        <v>229</v>
+      </c>
+      <c r="G54" t="s" s="15">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="55" ht="60.0" customHeight="true">
+      <c r="B55" t="s" s="13">
+        <v>231</v>
+      </c>
+      <c r="C55" t="s" s="14">
+        <v>232</v>
+      </c>
+      <c r="D55" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E55" t="s" s="17">
+        <v>233</v>
+      </c>
+      <c r="F55" t="s" s="16">
+        <v>234</v>
+      </c>
+      <c r="G55" t="s" s="15">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="56" ht="60.0" customHeight="true">
+      <c r="B56" t="s" s="13">
+        <v>236</v>
+      </c>
+      <c r="C56" t="s" s="14">
+        <v>237</v>
+      </c>
+      <c r="D56" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E56" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="F56" t="s" s="16">
+        <v>238</v>
+      </c>
+      <c r="G56" t="s" s="15">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="57" ht="60.0" customHeight="true">
+      <c r="B57" t="s" s="13">
+        <v>240</v>
+      </c>
+      <c r="C57" t="s" s="14">
+        <v>241</v>
+      </c>
+      <c r="D57" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E57" t="s" s="17">
+        <v>242</v>
+      </c>
+      <c r="F57" t="s" s="16">
+        <v>243</v>
+      </c>
+      <c r="G57" t="s" s="15">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" ht="60.0" customHeight="true">
+      <c r="B58" t="s" s="13">
+        <v>245</v>
+      </c>
+      <c r="C58" t="s" s="14">
+        <v>246</v>
+      </c>
+      <c r="D58" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E58" t="s" s="17">
+        <v>247</v>
+      </c>
+      <c r="F58" t="s" s="16">
+        <v>248</v>
+      </c>
+      <c r="G58" t="s" s="15">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="59" ht="60.0" customHeight="true">
+      <c r="B59" t="s" s="13">
+        <v>250</v>
+      </c>
+      <c r="C59" t="s" s="14">
+        <v>251</v>
+      </c>
+      <c r="D59" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E59" t="s" s="17">
+        <v>103</v>
+      </c>
+      <c r="F59" t="s" s="16">
+        <v>252</v>
+      </c>
+      <c r="G59" t="s" s="15">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" ht="60.0" customHeight="true">
+      <c r="B60" t="s" s="13">
+        <v>254</v>
+      </c>
+      <c r="C60" t="s" s="14">
+        <v>255</v>
+      </c>
+      <c r="D60" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E60" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="F60" t="s" s="16">
+        <v>256</v>
+      </c>
+      <c r="G60" t="s" s="15">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" ht="60.0" customHeight="true">
+      <c r="B61" t="s" s="13">
+        <v>258</v>
+      </c>
+      <c r="C61" t="s" s="14">
+        <v>259</v>
+      </c>
+      <c r="D61" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E61" t="s" s="17">
+        <v>124</v>
+      </c>
+      <c r="F61" t="s" s="16">
+        <v>260</v>
+      </c>
+      <c r="G61" t="s" s="15">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="62" ht="60.0" customHeight="true">
+      <c r="B62" t="s" s="13">
+        <v>262</v>
+      </c>
+      <c r="C62" t="s" s="14">
+        <v>263</v>
+      </c>
+      <c r="D62" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E62" t="s" s="17">
+        <v>68</v>
+      </c>
+      <c r="F62" t="s" s="16">
+        <v>264</v>
+      </c>
+      <c r="G62" t="s" s="15">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="63" ht="60.0" customHeight="true">
+      <c r="B63" t="s" s="13">
+        <v>266</v>
+      </c>
+      <c r="C63" t="s" s="14">
+        <v>267</v>
+      </c>
+      <c r="D63" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E63" t="s" s="17">
+        <v>79</v>
+      </c>
+      <c r="F63" t="s" s="16">
+        <v>268</v>
+      </c>
+      <c r="G63" t="s" s="15">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="64" ht="60.0" customHeight="true">
+      <c r="B64" t="s" s="13">
+        <v>270</v>
+      </c>
+      <c r="C64" t="s" s="14">
+        <v>271</v>
+      </c>
+      <c r="D64" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E64" t="s" s="17">
+        <v>272</v>
+      </c>
+      <c r="F64" t="s" s="16">
+        <v>273</v>
+      </c>
+      <c r="G64" t="s" s="15">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="65" ht="60.0" customHeight="true">
+      <c r="B65" t="s" s="13">
+        <v>275</v>
+      </c>
+      <c r="C65" t="s" s="14">
+        <v>276</v>
+      </c>
+      <c r="D65" t="s" s="16">
+        <v>272</v>
+      </c>
+      <c r="E65" t="s" s="17">
+        <v>47</v>
+      </c>
+      <c r="F65" t="s" s="16">
+        <v>268</v>
+      </c>
+      <c r="G65" t="s" s="15">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="66" ht="60.0" customHeight="true">
+      <c r="B66" t="s" s="13">
+        <v>278</v>
+      </c>
+      <c r="C66" t="s" s="14">
+        <v>279</v>
+      </c>
+      <c r="D66" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E66" t="s" s="17">
+        <v>103</v>
+      </c>
+      <c r="F66" t="s" s="16">
+        <v>280</v>
+      </c>
+      <c r="G66" t="s" s="15">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="67" ht="60.0" customHeight="true">
+      <c r="B67" t="s" s="13">
+        <v>282</v>
+      </c>
+      <c r="C67" t="s" s="14">
+        <v>283</v>
+      </c>
+      <c r="D67" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E67" t="s" s="17">
+        <v>284</v>
+      </c>
+      <c r="F67" t="s" s="16">
+        <v>285</v>
+      </c>
+      <c r="G67" t="s" s="15">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="68" ht="60.0" customHeight="true">
+      <c r="B68" t="s" s="13">
+        <v>287</v>
+      </c>
+      <c r="C68" t="s" s="14">
+        <v>288</v>
+      </c>
+      <c r="D68" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E68" t="s" s="17">
+        <v>124</v>
+      </c>
+      <c r="F68" t="s" s="16">
+        <v>289</v>
+      </c>
+      <c r="G68" t="s" s="15">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="69" ht="60.0" customHeight="true">
+      <c r="B69" t="s" s="13">
+        <v>291</v>
+      </c>
+      <c r="C69" t="s" s="14">
+        <v>292</v>
+      </c>
+      <c r="D69" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E69" t="s" s="17">
+        <v>293</v>
+      </c>
+      <c r="F69" t="s" s="16">
+        <v>294</v>
+      </c>
+      <c r="G69" t="s" s="15">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="70" ht="60.0" customHeight="true">
+      <c r="B70" t="s" s="13">
+        <v>296</v>
+      </c>
+      <c r="C70" t="s" s="14">
+        <v>297</v>
+      </c>
+      <c r="D70" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E70" t="s" s="17">
+        <v>298</v>
+      </c>
+      <c r="F70" t="s" s="16">
+        <v>299</v>
+      </c>
+      <c r="G70" t="s" s="15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="71" ht="15.0" customHeight="true">
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" ht="19.5" customHeight="true">
+      <c r="B72" t="s" s="23">
+        <v>19</v>
+      </c>
+      <c r="C72" s="23"/>
+      <c r="D72" s="8"/>
+      <c r="E72" t="s" s="24">
+        <v>301</v>
+      </c>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
+    </row>
+    <row r="73" ht="15.0" customHeight="true">
+      <c r="B73" t="s" s="23">
+        <v>20</v>
+      </c>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" t="s" s="24">
+        <v>302</v>
+      </c>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
+    </row>
+    <row r="74" ht="10.5" customHeight="true">
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+    </row>
+    <row r="75" ht="16.9" customHeight="true">
+      <c r="B75" t="s" s="20">
         <v>1</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+    </row>
+    <row r="76" ht="13.9" customHeight="true">
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="21"/>
+    </row>
+    <row r="77" ht="21.0" customHeight="true">
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+    </row>
+    <row r="78" ht="13.9" customHeight="true">
+      <c r="B78" t="s" s="22">
+        <v>2</v>
+      </c>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="22"/>
+      <c r="G78" s="22"/>
+    </row>
+    <row r="79" ht="18.0" customHeight="true">
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+    </row>
+    <row r="80" ht="12.0" customHeight="true">
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="22"/>
+    </row>
+    <row r="81" ht="13.15" customHeight="true">
+      <c r="B81" t="s" s="18">
+        <v>21</v>
+      </c>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+    </row>
+    <row r="82" ht="15.0" customHeight="true">
+      <c r="B82" s="18"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
+    </row>
+    <row r="83" ht="26.25" customHeight="true">
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+    </row>
+    <row r="84" ht="8.25" customHeight="true">
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+    </row>
+    <row r="85" ht="15.0" customHeight="true">
+      <c r="B85" t="s" s="19">
+        <v>22</v>
+      </c>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="19"/>
+    </row>
+    <row r="86" ht="15.0" customHeight="true">
+      <c r="B86" s="19"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
+    </row>
+    <row r="87" ht="15.0" customHeight="true">
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B40:G42"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B30:G32"/>
-    <mergeCell ref="B33:G35"/>
-    <mergeCell ref="B36:G38"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B75:G77"/>
+    <mergeCell ref="B78:G80"/>
+    <mergeCell ref="B81:G83"/>
+    <mergeCell ref="B85:G87"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E73:G73"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>